<commit_message>
update bode plots; add phasengang diagram; insert grenzfrequenz in bode plots
</commit_message>
<xml_diff>
--- a/lu2/aufgabe3.1_rc_tiefpass_bodediagramm.xlsx
+++ b/lu2/aufgabe3.1_rc_tiefpass_bodediagramm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="13260" activeTab="4"/>
+    <workbookView windowWidth="24292" windowHeight="13042" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,12 +99,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,7 +116,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -128,31 +128,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,6 +152,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,7 +183,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,30 +220,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,30 +244,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,7 +266,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,19 +392,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,151 +440,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,6 +480,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,30 +534,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -564,153 +548,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -718,60 +711,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -801,10 +794,11 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -816,10 +810,12 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -835,18 +831,21 @@
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:ln w="9525">
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                   <a:noFill/>
+                  <a:prstDash val="solid"/>
+                  <a:round/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
@@ -942,6 +941,32 @@
                 </c:rich>
               </c:tx>
               <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1029,6 +1054,7 @@
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:prstDash val="solid"/>
                       <a:round/>
                     </a:ln>
                     <a:effectLst/>
@@ -1193,12 +1219,13 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="9525" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1365,7 +1392,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:spPr>
-            <a:ln w="12700" cap="rnd" cmpd="sng">
+            <a:ln w="12700" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent5">
                   <a:alpha val="86000"/>
@@ -1383,10 +1410,12 @@
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent5"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1547,7 +1576,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1569,7 +1597,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -1577,6 +1604,7 @@
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1591,6 +1619,7 @@
                   <a:lumOff val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1646,6 +1675,7 @@
                 <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="solid"/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -1683,7 +1713,6 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -1691,6 +1720,7 @@
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1746,6 +1776,7 @@
                 <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="solid"/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -1796,6 +1827,7 @@
           <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:prstDash val="solid"/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1811,7 +1843,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2347,7 +2379,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2369,7 +2400,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -2499,7 +2529,6 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -2627,7 +2656,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3172,7 +3201,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3194,7 +3222,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -3309,7 +3336,6 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -3437,7 +3463,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3940,7 +3966,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3962,7 +3987,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4076,7 +4100,6 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4204,7 +4227,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4413,7 +4436,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4435,7 +4457,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4549,7 +4570,6 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4677,7 +4697,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4993,10 +5013,12 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
+            <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -5004,13 +5026,183 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="24"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="25"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="26"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="27"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="28"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="29"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="30"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="31"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="32"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="33"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="34"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="35"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="36"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="37"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="38"/>
+              <c:delete val="1"/>
+            </c:dLbl>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr lang="de-AT" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
@@ -5028,8 +5220,10 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln>
+                    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                       <a:noFill/>
+                      <a:prstDash val="solid"/>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -5039,10 +5233,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$H$2:$H$40</c:f>
+              <c:f>Sheet3!$H$2:$H$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="1">
                   <c:v>15800</c:v>
                 </c:pt>
@@ -5155,6 +5349,9 @@
                   <c:v>15800</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>15800</c:v>
                 </c:pt>
               </c:numCache>
@@ -5162,10 +5359,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$G$2:$G$40</c:f>
+              <c:f>Sheet3!$G$2:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5279,6 +5476,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5286,7 +5486,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -5309,7 +5508,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -5325,7 +5523,6 @@
         </c:majorGridlines>
         <c:minorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -5443,13 +5640,13 @@
         <c:axId val="751046084"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="15"/>
           <c:min val="-40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -5609,7 +5806,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5649,7 +5846,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -5907,8 +6104,276 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$H$3:$H$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$D$3:$D$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-7.23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-10.31</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-15.03</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-17.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-31.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-37.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-44.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-54.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-66.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-81.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-92.13</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-96.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-121.3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-130.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-137.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-146.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-152.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-165.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-169.3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-171.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-172.3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-173.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-175.3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-176.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-178</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-181.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-184</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -5930,7 +6395,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -6038,12 +6502,13 @@
         <c:axId val="94895867"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="-190"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -6171,7 +6636,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6457,10 +6922,12 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
+            <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -6468,13 +6935,163 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="24"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="25"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="26"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="27"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="28"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="29"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="30"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="31"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="32"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="33"/>
+              <c:delete val="1"/>
+            </c:dLbl>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr lang="de-AT" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
@@ -6492,8 +7109,10 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln>
+                    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                       <a:noFill/>
+                      <a:prstDash val="solid"/>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -6726,7 +7345,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -6749,7 +7367,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -6765,7 +7382,6 @@
         </c:majorGridlines>
         <c:minorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -6883,12 +7499,13 @@
         <c:axId val="713527484"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="-30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -7048,7 +7665,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7088,7 +7705,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -7299,13 +7916,243 @@
                 <c:pt idx="27">
                   <c:v>-157.87</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>-180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$H$2:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$D$3:$D$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6.43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-12.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-25.32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-49.78</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-61.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-66.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-71.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-76</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-83.23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-88.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-91.87</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-92.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-95.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-98.07</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-105.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-119.45</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-126</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-135.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-142.53</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-146</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-155.3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-157.87</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-180</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -7327,7 +8174,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -7440,7 +8286,6 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -7568,7 +8413,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7592,7 +8437,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="line"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
@@ -7609,13 +8454,12 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FFC000"/>
-            </a:solidFill>
-            <a:ln w="28575">
+            <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -7623,13 +8467,179 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="24"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="25"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="26"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="27"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="28"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="29"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="30"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="31"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="32"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="33"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="34"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="35"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="36"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="37"/>
+              <c:delete val="1"/>
+            </c:dLbl>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr lang="de-AT" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
@@ -7647,8 +8657,10 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln>
+                    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                       <a:noFill/>
+                      <a:prstDash val="solid"/>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -8194,15 +9206,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FFC000"/>
-            </a:solidFill>
-            <a:ln w="28575">
+            <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent6">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -8210,13 +9221,179 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="24"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="25"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="26"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="27"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="28"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="29"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="30"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="31"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="32"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="33"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="34"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="35"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="36"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="37"/>
+              <c:delete val="1"/>
+            </c:dLbl>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr lang="de-AT" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
@@ -8234,8 +9411,10 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln>
+                    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                       <a:noFill/>
+                      <a:prstDash val="solid"/>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -8492,7 +9671,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -8514,7 +9692,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -8530,7 +9707,6 @@
         </c:majorGridlines>
         <c:minorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -8654,7 +9830,6 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -8814,7 +9989,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9092,13 +10267,521 @@
                 <c:pt idx="31">
                   <c:v>-147</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>-180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet5!$I$3:$I$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>145000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet5!$D$3:$D$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>-0.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-17.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-23.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-28.63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-29.15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-31.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-34.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-39.34</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-42.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-44</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-48</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-50.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-53.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-57.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-62.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-68.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-76</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-83</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-104</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-114</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-124</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-130</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-134</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-138</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-147</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet5!$H$3:$H$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1610</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet5!$D$3:$D$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>-0.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-17.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-23.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-28.63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-29.15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-31.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-34.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-39.34</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-42.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-44</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-48</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-50.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-53.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-57.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-62.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-68.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-76</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-83</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-104</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-114</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-124</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-130</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-134</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-138</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-147</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-180</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -9120,7 +10803,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -9228,12 +10910,12 @@
         <c:axId val="544951191"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-180"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -9361,7 +11043,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9918,7 +11600,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -9940,7 +11621,6 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -10054,7 +11734,6 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -10198,17 +11877,17 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -10242,10 +11921,13 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -10518,46 +12200,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -14171,522 +15813,6 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15223,8 +16349,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10617835" y="419100"/>
-        <a:ext cx="8543925" cy="3081020"/>
+        <a:off x="8042275" y="457200"/>
+        <a:ext cx="6423025" cy="3442970"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15253,8 +16379,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10569575" y="3738880"/>
-        <a:ext cx="8573135" cy="2766060"/>
+        <a:off x="7994015" y="4177030"/>
+        <a:ext cx="6452235" cy="3089910"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15288,8 +16414,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9001760" y="269875"/>
-        <a:ext cx="8366760" cy="3381375"/>
+        <a:off x="6897370" y="288925"/>
+        <a:ext cx="6245860" cy="3781425"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15308,7 +16434,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:colOff>236855</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>151765</xdr:rowOff>
     </xdr:to>
@@ -15318,8 +16444,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9029065" y="3752850"/>
-        <a:ext cx="8323580" cy="3199765"/>
+        <a:off x="6924675" y="4191000"/>
+        <a:ext cx="6217285" cy="3561715"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15337,13 +16463,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>793750</xdr:colOff>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>786130</xdr:colOff>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>110490</xdr:rowOff>
     </xdr:to>
@@ -15353,8 +16479,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9761855" y="266700"/>
-        <a:ext cx="8590280" cy="3082290"/>
+        <a:off x="7404100" y="285750"/>
+        <a:ext cx="6477000" cy="3444240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15383,8 +16509,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9847580" y="3536315"/>
-        <a:ext cx="8359140" cy="3230880"/>
+        <a:off x="7423785" y="3936365"/>
+        <a:ext cx="6450330" cy="3611880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15408,7 +16534,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>777875</xdr:colOff>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:to>
@@ -15418,8 +16544,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8680450" y="308610"/>
-        <a:ext cx="8368030" cy="3101975"/>
+        <a:off x="6576060" y="327660"/>
+        <a:ext cx="6329045" cy="3482975"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15432,15 +16558,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>461645</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>147955</xdr:rowOff>
+      <xdr:colOff>176530</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>10795</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>584835</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>120015</xdr:rowOff>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15448,8 +16574,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8994140" y="3548380"/>
-        <a:ext cx="8358505" cy="3048635"/>
+        <a:off x="6604635" y="3992245"/>
+        <a:ext cx="6237605" cy="3410585"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15475,7 +16601,7 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>643255</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>172720</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15483,8 +16609,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10479405" y="323850"/>
-        <a:ext cx="8639175" cy="3076575"/>
+        <a:off x="8042910" y="361950"/>
+        <a:ext cx="6518275" cy="3419475"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15499,7 +16625,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>17145</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
@@ -15513,8 +16639,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10754360" y="3562350"/>
-        <a:ext cx="8592820" cy="3237230"/>
+        <a:off x="8105775" y="3962400"/>
+        <a:ext cx="6471920" cy="3618230"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15548,8 +16674,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8675370" y="344170"/>
-        <a:ext cx="8361680" cy="3341370"/>
+        <a:off x="6539230" y="382270"/>
+        <a:ext cx="6452870" cy="3722370"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15570,7 +16696,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>176530</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15578,8 +16704,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8679815" y="3914775"/>
-        <a:ext cx="8578850" cy="3209925"/>
+        <a:off x="6543675" y="4371975"/>
+        <a:ext cx="6457950" cy="3571875"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15597,7 +16723,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="4A4A4A"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -15844,7 +16970,6 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -15857,9 +16982,9 @@
       <selection activeCell="A24" sqref="A3:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
-    <col min="5" max="5" width="12.7933333333333"/>
+    <col min="5" max="5" width="12.7964601769912"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -16289,12 +17414,12 @@
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="13.86"/>
-    <col min="5" max="5" width="13.86"/>
-    <col min="7" max="7" width="13.86"/>
-    <col min="9" max="9" width="13.86"/>
+    <col min="2" max="2" width="13.858407079646"/>
+    <col min="5" max="5" width="13.858407079646"/>
+    <col min="7" max="7" width="13.858407079646"/>
+    <col min="9" max="9" width="13.858407079646"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -16926,16 +18051,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="5" max="5" width="12.7933333333333"/>
-    <col min="7" max="7" width="13.6"/>
+    <col min="5" max="5" width="12.7964601769912"/>
+    <col min="7" max="7" width="13.6017699115044"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -17885,11 +19010,22 @@
         <v>15800</v>
       </c>
     </row>
-    <row r="40" spans="7:8">
+    <row r="40" spans="4:8">
+      <c r="D40">
+        <v>-190</v>
+      </c>
       <c r="G40">
         <v>-40</v>
       </c>
       <c r="H40" s="1">
+        <v>15800</v>
+      </c>
+    </row>
+    <row r="41" spans="7:8">
+      <c r="G41">
+        <v>15</v>
+      </c>
+      <c r="H41">
         <v>15800</v>
       </c>
     </row>
@@ -17906,13 +19042,13 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="5" max="5" width="12.7933333333333"/>
-    <col min="6" max="7" width="13.6"/>
+    <col min="5" max="5" width="12.7964601769912"/>
+    <col min="6" max="7" width="13.6017699115044"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -18652,6 +19788,9 @@
       </c>
       <c r="C31">
         <v>0.075</v>
+      </c>
+      <c r="D31">
+        <v>-180</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
@@ -18751,14 +19890,14 @@
   <sheetPr/>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="12.7933333333333"/>
-    <col min="7" max="7" width="13.6"/>
+    <col min="5" max="5" width="12.7964601769912"/>
+    <col min="7" max="7" width="13.6017699115044"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -19686,6 +20825,9 @@
       <c r="C35">
         <v>0.014</v>
       </c>
+      <c r="D35">
+        <v>-180</v>
+      </c>
       <c r="E35">
         <f t="shared" si="0"/>
         <v>0.0142131979695431</v>
@@ -19711,6 +20853,7 @@
       <c r="C36">
         <v>0.013</v>
       </c>
+      <c r="D36"/>
       <c r="E36">
         <f t="shared" si="0"/>
         <v>0.0131578947368421</v>
@@ -19736,6 +20879,7 @@
       <c r="C37">
         <v>0.01</v>
       </c>
+      <c r="D37"/>
       <c r="E37">
         <f t="shared" si="0"/>
         <v>0.0100502512562814</v>
@@ -19828,11 +20972,11 @@
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="12.7933333333333"/>
-    <col min="6" max="6" width="13.86"/>
-    <col min="8" max="8" width="13.86"/>
+    <col min="5" max="5" width="12.7964601769912"/>
+    <col min="6" max="6" width="13.858407079646"/>
+    <col min="8" max="8" width="13.858407079646"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -20622,9 +21766,9 @@
       <selection activeCell="U47" sqref="U47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="5" max="6" width="13.86"/>
+    <col min="5" max="6" width="13.858407079646"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">

</xml_diff>

<commit_message>
mein teil is jez mehr oder weniger fertig. die messdaten measma nu hinzufuegen!
</commit_message>
<xml_diff>
--- a/lu2/aufgabe3.1_rc_tiefpass_bodediagramm.xlsx
+++ b/lu2/aufgabe3.1_rc_tiefpass_bodediagramm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24292" windowHeight="13042" activeTab="2"/>
+    <workbookView windowWidth="24300" windowHeight="13260" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,10 +99,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -121,14 +121,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -136,9 +128,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -152,28 +196,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,15 +205,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,31 +227,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,15 +249,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,13 +266,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,13 +344,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +374,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,49 +416,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,85 +440,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,26 +460,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -519,17 +519,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,162 +557,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -717,54 +717,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -794,6 +794,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -841,6 +842,7 @@
             </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
+              <a:noFill/>
               <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
@@ -916,7 +918,7 @@
                   <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:pPr defTabSz="914400">
+                    <a:pPr algn="ctr" defTabSz="914400">
                       <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
                           <a:schemeClr val="tx1">
@@ -948,25 +950,6 @@
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1047,6 +1030,7 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
+                    <a:noFill/>
                     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
@@ -1219,6 +1203,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2">
@@ -1392,6 +1377,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="12700" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent5">
@@ -1576,6 +1562,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1597,6 +1584,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -1612,6 +1600,7 @@
         </c:majorGridlines>
         <c:minorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -1713,6 +1702,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -1843,7 +1833,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2379,6 +2369,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2400,6 +2391,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -2529,6 +2521,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -2656,7 +2649,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3201,6 +3194,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3222,6 +3216,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -3336,6 +3331,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -3463,7 +3459,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3966,6 +3962,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3987,6 +3984,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4100,6 +4098,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4227,7 +4226,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4436,6 +4435,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4457,6 +4457,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4570,6 +4571,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -4697,7 +4699,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4727,6 +4729,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -5013,6 +5016,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -5220,6 +5224,7 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
+                    <a:noFill/>
                     <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                       <a:noFill/>
                       <a:prstDash val="solid"/>
@@ -5486,6 +5491,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -5508,6 +5514,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -5523,6 +5530,7 @@
         </c:majorGridlines>
         <c:minorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -5647,6 +5655,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -5806,7 +5815,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6374,6 +6383,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -6395,6 +6405,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -6509,6 +6520,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -6636,7 +6648,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6666,6 +6678,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -6922,6 +6935,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -7109,6 +7123,7 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
+                    <a:noFill/>
                     <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                       <a:noFill/>
                       <a:prstDash val="solid"/>
@@ -7345,6 +7360,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -7367,6 +7383,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -7382,6 +7399,7 @@
         </c:majorGridlines>
         <c:minorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -7506,6 +7524,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -7665,7 +7684,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8153,6 +8172,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -8174,6 +8194,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -8286,6 +8307,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -8413,7 +8435,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8454,6 +8476,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -8657,6 +8680,7 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
+                    <a:noFill/>
                     <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                       <a:noFill/>
                       <a:prstDash val="solid"/>
@@ -8920,6 +8944,7 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -9206,6 +9231,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent6">
@@ -9411,6 +9437,7 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
+                    <a:noFill/>
                     <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
                       <a:noFill/>
                       <a:prstDash val="solid"/>
@@ -9671,6 +9698,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -9692,6 +9720,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -9707,6 +9736,7 @@
         </c:majorGridlines>
         <c:minorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -9830,6 +9860,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -9989,7 +10020,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10047,10 +10078,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet5!$A$3:$A$39</c:f>
+              <c:f>Sheet5!$A$3:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -10152,25 +10183,16 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>150000</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>200000</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet5!$D$3:$D$39</c:f>
+              <c:f>Sheet5!$D$3:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>-0.41</c:v>
                 </c:pt>
@@ -10265,10 +10287,13 @@
                   <c:v>-138</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>-142</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>-147</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>-180</c:v>
+                <c:pt idx="33">
+                  <c:v>-150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10298,10 +10323,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet5!$I$3:$I$40</c:f>
+              <c:f>Sheet5!$I$3:$I$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>145000</c:v>
                 </c:pt>
@@ -10402,18 +10427,6 @@
                   <c:v>145000</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>145000</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>145000</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>145000</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>145000</c:v>
-                </c:pt>
-                <c:pt idx="37">
                   <c:v>145000</c:v>
                 </c:pt>
               </c:numCache>
@@ -10421,10 +10434,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet5!$D$3:$D$40</c:f>
+              <c:f>Sheet5!$D$3:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>-0.41</c:v>
                 </c:pt>
@@ -10519,10 +10532,13 @@
                   <c:v>-138</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>-142</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>-147</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>-180</c:v>
+                <c:pt idx="33">
+                  <c:v>-150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10550,10 +10566,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet5!$H$3:$H$40</c:f>
+              <c:f>Sheet5!$H$3:$H$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>1610</c:v>
                 </c:pt>
@@ -10654,18 +10670,6 @@
                   <c:v>1610</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1610</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1610</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1610</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1610</c:v>
-                </c:pt>
-                <c:pt idx="37">
                   <c:v>1610</c:v>
                 </c:pt>
               </c:numCache>
@@ -10673,10 +10677,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet5!$D$3:$D$40</c:f>
+              <c:f>Sheet5!$D$3:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>-0.41</c:v>
                 </c:pt>
@@ -10771,10 +10775,13 @@
                   <c:v>-138</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>-142</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>-147</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>-180</c:v>
+                <c:pt idx="33">
+                  <c:v>-150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10782,6 +10789,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -10803,6 +10811,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -10869,7 +10878,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -10910,12 +10919,13 @@
         <c:axId val="544951191"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-180"/>
+          <c:min val="-150"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -11043,7 +11053,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11600,6 +11610,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -11621,6 +11632,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -11734,6 +11746,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
+            <a:noFill/>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -11877,7 +11890,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -16349,8 +16362,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8042275" y="457200"/>
-        <a:ext cx="6423025" cy="3442970"/>
+        <a:off x="10617835" y="419100"/>
+        <a:ext cx="8543925" cy="3081020"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16379,8 +16392,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7994015" y="4177030"/>
-        <a:ext cx="6452235" cy="3089910"/>
+        <a:off x="10569575" y="3738880"/>
+        <a:ext cx="8573135" cy="2766060"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16414,8 +16427,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6897370" y="288925"/>
-        <a:ext cx="6245860" cy="3781425"/>
+        <a:off x="9001760" y="269875"/>
+        <a:ext cx="8366760" cy="3381375"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16444,8 +16457,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6924675" y="4191000"/>
-        <a:ext cx="6217285" cy="3561715"/>
+        <a:off x="9029065" y="3752850"/>
+        <a:ext cx="8338185" cy="3199765"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16479,8 +16492,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7404100" y="285750"/>
-        <a:ext cx="6477000" cy="3444240"/>
+        <a:off x="9615805" y="266700"/>
+        <a:ext cx="8597900" cy="3082290"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16509,8 +16522,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7423785" y="3936365"/>
-        <a:ext cx="6450330" cy="3611880"/>
+        <a:off x="9847580" y="3536315"/>
+        <a:ext cx="8359140" cy="3230880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16544,8 +16557,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6576060" y="327660"/>
-        <a:ext cx="6329045" cy="3482975"/>
+        <a:off x="8680450" y="308610"/>
+        <a:ext cx="8237855" cy="3101975"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16558,15 +16571,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>176530</xdr:colOff>
+      <xdr:colOff>168275</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>10795</xdr:rowOff>
+      <xdr:rowOff>10160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>584835</xdr:colOff>
+      <xdr:colOff>576580</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:rowOff>161290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16574,8 +16587,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6604635" y="3992245"/>
-        <a:ext cx="6237605" cy="3410585"/>
+        <a:off x="8700770" y="3572510"/>
+        <a:ext cx="8146415" cy="3065780"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16609,8 +16622,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8042910" y="361950"/>
-        <a:ext cx="6518275" cy="3419475"/>
+        <a:off x="10479405" y="323850"/>
+        <a:ext cx="8639175" cy="3076575"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16639,8 +16652,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8105775" y="3962400"/>
-        <a:ext cx="6471920" cy="3618230"/>
+        <a:off x="10754360" y="3562350"/>
+        <a:ext cx="8592820" cy="3237230"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16674,8 +16687,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6539230" y="382270"/>
-        <a:ext cx="6452870" cy="3722370"/>
+        <a:off x="8675370" y="344170"/>
+        <a:ext cx="8361680" cy="3341370"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16704,8 +16717,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6543675" y="4371975"/>
-        <a:ext cx="6457950" cy="3571875"/>
+        <a:off x="8679815" y="3914775"/>
+        <a:ext cx="8578850" cy="3209925"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16723,7 +16736,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="4A4A4A"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -16970,6 +16983,7 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -16982,9 +16996,9 @@
       <selection activeCell="A24" sqref="A3:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
-    <col min="5" max="5" width="12.7964601769912"/>
+    <col min="5" max="5" width="12.7933333333333"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -17414,12 +17428,12 @@
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="13.858407079646"/>
-    <col min="5" max="5" width="13.858407079646"/>
-    <col min="7" max="7" width="13.858407079646"/>
-    <col min="9" max="9" width="13.858407079646"/>
+    <col min="2" max="2" width="13.86"/>
+    <col min="5" max="5" width="13.86"/>
+    <col min="7" max="7" width="13.86"/>
+    <col min="9" max="9" width="13.86"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -18053,14 +18067,14 @@
   <sheetPr/>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <cols>
-    <col min="5" max="5" width="12.7964601769912"/>
-    <col min="7" max="7" width="13.6017699115044"/>
+    <col min="5" max="5" width="12.7933333333333"/>
+    <col min="7" max="7" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -19041,14 +19055,14 @@
   <sheetPr/>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <cols>
-    <col min="5" max="5" width="12.7964601769912"/>
-    <col min="6" max="7" width="13.6017699115044"/>
+    <col min="5" max="5" width="12.7933333333333"/>
+    <col min="6" max="7" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -19890,14 +19904,14 @@
   <sheetPr/>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75"/>
   <cols>
-    <col min="5" max="5" width="12.7964601769912"/>
-    <col min="7" max="7" width="13.6017699115044"/>
+    <col min="5" max="5" width="12.7933333333333"/>
+    <col min="7" max="7" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -20798,7 +20812,7 @@
         <v>0.015</v>
       </c>
       <c r="D34">
-        <v>-147</v>
+        <v>-142</v>
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
@@ -20826,7 +20840,7 @@
         <v>0.014</v>
       </c>
       <c r="D35">
-        <v>-180</v>
+        <v>-147</v>
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
@@ -20853,7 +20867,9 @@
       <c r="C36">
         <v>0.013</v>
       </c>
-      <c r="D36"/>
+      <c r="D36">
+        <v>-150</v>
+      </c>
       <c r="E36">
         <f t="shared" si="0"/>
         <v>0.0131578947368421</v>
@@ -20879,7 +20895,6 @@
       <c r="C37">
         <v>0.01</v>
       </c>
-      <c r="D37"/>
       <c r="E37">
         <f t="shared" si="0"/>
         <v>0.0100502512562814</v>
@@ -20972,11 +20987,11 @@
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75"/>
   <cols>
-    <col min="5" max="5" width="12.7964601769912"/>
-    <col min="6" max="6" width="13.858407079646"/>
-    <col min="8" max="8" width="13.858407079646"/>
+    <col min="5" max="5" width="12.7933333333333"/>
+    <col min="6" max="6" width="13.86"/>
+    <col min="8" max="8" width="13.86"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -21766,9 +21781,9 @@
       <selection activeCell="U47" sqref="U47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.02666666666667" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <cols>
-    <col min="5" max="6" width="13.858407079646"/>
+    <col min="5" max="6" width="13.86"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">

</xml_diff>